<commit_message>
[LLgrammar] grammar.txt update, LLtable update
</commit_message>
<xml_diff>
--- a/docs/LLtable.xlsx
+++ b/docs/LLtable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\5 semester\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\5 semester\IFJ [Formal Languages and Compilers]\project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAC26F21-46D8-472F-AD4E-7F04BE9918D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6443D25B-1E13-417B-90CB-50A02A11E4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{737553C5-0C24-438F-A3BF-0ACBB334197E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>&lt;program&gt;</t>
   </si>
@@ -134,16 +134,19 @@
     <t>$id</t>
   </si>
   <si>
-    <t>"string"</t>
-  </si>
-  <si>
     <t>void</t>
   </si>
   <si>
     <t>%</t>
   </si>
   <si>
-    <t>32, 33</t>
+    <t>&lt;var_def_expr&gt;</t>
+  </si>
+  <si>
+    <t>"str"</t>
+  </si>
+  <si>
+    <t>&lt;expr&gt;</t>
   </si>
 </sst>
 </file>
@@ -510,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20486AAE-D447-4BD7-B206-7D2617A59371}">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +526,7 @@
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
@@ -570,16 +573,19 @@
         <v>30</v>
       </c>
       <c r="Q1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" t="s">
         <v>32</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +610,7 @@
       <c r="R2" s="3"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -629,7 +635,7 @@
       <c r="R3" s="3"/>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -666,7 +672,7 @@
       <c r="R4" s="3"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -701,7 +707,7 @@
       <c r="R5" s="3"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -725,8 +731,11 @@
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="1"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -751,7 +760,7 @@
       <c r="R7" s="3"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -767,7 +776,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
@@ -776,7 +785,7 @@
       <c r="R8" s="3"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -786,7 +795,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -801,7 +810,7 @@
       <c r="R9" s="3"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -817,22 +826,20 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R10" s="3"/>
-      <c r="S10" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -848,18 +855,18 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="R11" s="3"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -877,18 +884,16 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3">
+        <v>23</v>
+      </c>
+      <c r="P12" s="3">
         <v>22</v>
-      </c>
-      <c r="P12" s="3">
-        <v>21</v>
       </c>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
-      <c r="S12" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -899,33 +904,31 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I13" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J13" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K13" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L13" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -936,19 +939,19 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I14" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J14" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K14" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L14" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -958,7 +961,7 @@
       <c r="R14" s="3"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -976,18 +979,16 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3">
-        <v>32</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="P15" s="3">
+        <v>34</v>
       </c>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
-      <c r="S15" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -998,19 +999,19 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I16" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J16" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K16" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L16" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -1020,7 +1021,7 @@
       <c r="R16" s="3"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1036,7 +1037,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
@@ -1045,7 +1046,7 @@
       <c r="R17" s="3"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1056,19 +1057,19 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I18" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J18" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K18" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L18" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -1076,12 +1077,20 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3">
+        <v>35</v>
+      </c>
+      <c r="S18" s="1"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S18" s="1"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="G19">
+        <v>15</v>
+      </c>
+      <c r="T19">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[general] scanner warnings fix, symtable implementation, updated project structure, created new modules todo
</commit_message>
<xml_diff>
--- a/docs/LLtable.xlsx
+++ b/docs/LLtable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\5 semester\IFJ [Formal Languages and Compilers]\project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6443D25B-1E13-417B-90CB-50A02A11E4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08B8071-AB10-4404-9116-0E29A7C69E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{737553C5-0C24-438F-A3BF-0ACBB334197E}"/>
   </bookViews>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20486AAE-D447-4BD7-B206-7D2617A59371}">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,10 +1085,27 @@
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G19">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1">
         <v>15</v>
       </c>
-      <c r="T19">
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1">
         <v>16</v>
       </c>
     </row>

</xml_diff>